<commit_message>
DDF2 add Data Provider(excel) and refactor TestBase code, add new TC
</commit_message>
<xml_diff>
--- a/DDFramework2/src/test/resources/excel/testdata.xlsx
+++ b/DDFramework2/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,33 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Email or Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user@phptravels.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi, Demo User</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alertText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M6B 123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -172,18 +169,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,92 +193,22 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DDF2 - add soft Assertions with screenshot
</commit_message>
<xml_diff>
--- a/DDFramework2/src/test/resources/excel/testdata.xlsx
+++ b/DDFramework2/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -44,6 +45,15 @@
   </si>
   <si>
     <t xml:space="preserve">Customer added successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dollars</t>
   </si>
 </sst>
 </file>
@@ -171,8 +181,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -220,4 +230,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DDF2 - add TC with Select and DataProvider
</commit_message>
<xml_diff>
--- a/DDFramework2/src/test/resources/excel/testdata.xlsx
+++ b/DDFramework2/src/test/resources/excel/testdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -53,7 +53,27 @@
     <t xml:space="preserve">currency</t>
   </si>
   <si>
-    <t xml:space="preserve">dollars</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Alex </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Go</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Dollar</t>
   </si>
 </sst>
 </file>
@@ -182,7 +202,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -240,7 +260,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -258,10 +278,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DDF2 - exclude TCs from test suite using TestSuite page in Excel file
</commit_message>
<xml_diff>
--- a/DDFramework2/src/test/resources/excel/testdata.xlsx
+++ b/DDFramework2/src/test/resources/excel/testdata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TestSuite" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="OpenAccountTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">TCID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RunMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginAsBankManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verifyTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addCustomerTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xtentExample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openAccountTest</t>
+  </si>
   <si>
     <t xml:space="preserve">firstName</t>
   </si>
@@ -170,15 +198,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,6 +227,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -207,38 +311,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="3" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="25.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -252,15 +356,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,19 +373,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>